<commit_message>
Actualizacion de listado de comunicacion
Actualizacion de listado de comunicacion
</commit_message>
<xml_diff>
--- a/2020/listados/Listado de medios de comunicacion con estudiantes.xlsx
+++ b/2020/listados/Listado de medios de comunicacion con estudiantes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\GitHub\liceopatria.github.io\2020\listados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB4823C-6001-4A2F-BC45-E2558F2174EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025DD072-4597-469C-948D-F15E9E05910A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8070" yWindow="1185" windowWidth="14400" windowHeight="10755" tabRatio="710" firstSheet="4" activeTab="6" xr2:uid="{50E3D567-1B3A-45B1-BFAB-81E44AF5B42C}"/>
+    <workbookView xWindow="4800" yWindow="1185" windowWidth="14400" windowHeight="10755" tabRatio="710" firstSheet="2" activeTab="3" xr2:uid="{50E3D567-1B3A-45B1-BFAB-81E44AF5B42C}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="15" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="517">
   <si>
     <t>Codigo</t>
   </si>
@@ -2817,13 +2817,13 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>27</c:v>
@@ -2841,7 +2841,7 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>32</c:v>
@@ -3009,13 +3009,13 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>7</c:v>
@@ -3033,7 +3033,7 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2</c:v>
@@ -3484,13 +3484,13 @@
                   <c:v>0.88235294117647056</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.44444444444444442</c:v>
+                  <c:v>0.47222222222222221</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.48484848484848486</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.76470588235294112</c:v>
+                  <c:v>0.79411764705882348</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.79411764705882348</c:v>
@@ -3508,7 +3508,7 @@
                   <c:v>0.59375</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.33333333333333331</c:v>
+                  <c:v>0.36363636363636365</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.94117647058823528</c:v>
@@ -3673,13 +3673,13 @@
                   <c:v>0.11764705882352941</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.55555555555555558</c:v>
+                  <c:v>0.52777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.51515151515151514</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.23529411764705882</c:v>
+                  <c:v>0.20588235294117646</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.20588235294117646</c:v>
@@ -3697,7 +3697,7 @@
                   <c:v>0.40625</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.66666666666666663</c:v>
+                  <c:v>0.63636363636363635</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>5.8823529411764705E-2</c:v>
@@ -5540,7 +5540,7 @@
       </c>
       <c r="D5" s="10">
         <f>'08-2'!D46</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="10">
         <f>'08-3'!D44</f>
@@ -5548,7 +5548,7 @@
       </c>
       <c r="F5" s="10">
         <f>'08-4'!D44</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G5" s="10">
         <f>'09-1'!D44</f>
@@ -5572,7 +5572,7 @@
       </c>
       <c r="L5" s="10">
         <f>'10-3'!D43</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M5" s="10">
         <f>'11-1'!D44</f>
@@ -5588,7 +5588,7 @@
       </c>
       <c r="P5" s="33">
         <f t="shared" ref="P5:P8" si="0">AVERAGE(B5:O5)</f>
-        <v>24.285714285714285</v>
+        <v>24.5</v>
       </c>
       <c r="Q5" s="33">
         <f t="shared" ref="Q5:Q8" si="1">MAX(B5:O5)</f>
@@ -5596,7 +5596,7 @@
       </c>
       <c r="R5" s="33">
         <f t="shared" ref="R5:R8" si="2">MIN(B5:O5)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
@@ -5613,7 +5613,7 @@
       </c>
       <c r="D6" s="10">
         <f>'08-2'!D47</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="10">
         <f>'08-3'!D45</f>
@@ -5621,7 +5621,7 @@
       </c>
       <c r="F6" s="10">
         <f>'08-4'!D45</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G6" s="10">
         <f>'09-1'!D45</f>
@@ -5645,7 +5645,7 @@
       </c>
       <c r="L6" s="10">
         <f>'10-3'!D44</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M6" s="10">
         <f>'11-1'!D45</f>
@@ -5661,11 +5661,11 @@
       </c>
       <c r="P6" s="33">
         <f t="shared" si="0"/>
-        <v>9.8571428571428577</v>
+        <v>9.6428571428571423</v>
       </c>
       <c r="Q6" s="33">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R6" s="33">
         <f t="shared" si="2"/>
@@ -5686,7 +5686,7 @@
       </c>
       <c r="D7" s="32">
         <f t="shared" si="3"/>
-        <v>0.44444444444444442</v>
+        <v>0.47222222222222221</v>
       </c>
       <c r="E7" s="32">
         <f t="shared" si="3"/>
@@ -5694,7 +5694,7 @@
       </c>
       <c r="F7" s="32">
         <f t="shared" si="3"/>
-        <v>0.76470588235294112</v>
+        <v>0.79411764705882348</v>
       </c>
       <c r="G7" s="32">
         <f t="shared" si="3"/>
@@ -5718,7 +5718,7 @@
       </c>
       <c r="L7" s="32">
         <f t="shared" si="3"/>
-        <v>0.33333333333333331</v>
+        <v>0.36363636363636365</v>
       </c>
       <c r="M7" s="32">
         <f t="shared" si="3"/>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="P7" s="34">
         <f t="shared" si="0"/>
-        <v>0.7148616643627147</v>
+        <v>0.72111113384747838</v>
       </c>
       <c r="Q7" s="34">
         <f t="shared" si="1"/>
@@ -5742,7 +5742,7 @@
       </c>
       <c r="R7" s="34">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
+        <v>0.36363636363636365</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
@@ -5759,7 +5759,7 @@
       </c>
       <c r="D8" s="36">
         <f t="shared" si="4"/>
-        <v>0.55555555555555558</v>
+        <v>0.52777777777777779</v>
       </c>
       <c r="E8" s="36">
         <f t="shared" si="4"/>
@@ -5767,7 +5767,7 @@
       </c>
       <c r="F8" s="36">
         <f t="shared" si="4"/>
-        <v>0.23529411764705882</v>
+        <v>0.20588235294117646</v>
       </c>
       <c r="G8" s="36">
         <f t="shared" si="4"/>
@@ -5791,7 +5791,7 @@
       </c>
       <c r="L8" s="36">
         <f t="shared" si="4"/>
-        <v>0.66666666666666663</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="M8" s="36">
         <f t="shared" si="4"/>
@@ -5807,11 +5807,11 @@
       </c>
       <c r="P8" s="37">
         <f t="shared" si="0"/>
-        <v>0.28513833563728519</v>
+        <v>0.27888886615252156</v>
       </c>
       <c r="Q8" s="37">
         <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="R8" s="37">
         <f t="shared" si="2"/>
@@ -7620,8 +7620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E6AB2A-DF13-43E5-8B37-FC6F541704E3}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7728,9 +7728,12 @@
       <c r="C7" s="9" t="s">
         <v>389</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -8221,7 +8224,7 @@
       <c r="C38" s="40"/>
       <c r="D38" s="22">
         <f>COUNTA(D5:D37)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E38" s="22">
         <f t="shared" ref="E38:G38" si="1">COUNTA(E5:E37)</f>
@@ -8237,7 +8240,7 @@
       </c>
       <c r="H38" s="23">
         <f>COUNTIF(H5:H37,"X")</f>
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -8271,11 +8274,11 @@
       </c>
       <c r="D43" s="10">
         <f>D42-D44</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E43" s="12">
         <f>D43/D42</f>
-        <v>0.33333333333333331</v>
+        <v>0.36363636363636365</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -8284,11 +8287,11 @@
       </c>
       <c r="D44" s="10">
         <f>H38</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E44" s="12">
         <f>D44/D42</f>
-        <v>0.66666666666666663</v>
+        <v>0.63636363636363635</v>
       </c>
     </row>
   </sheetData>
@@ -10583,7 +10586,7 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12176,8 +12179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50465DDD-5234-470A-A297-95DF11514D18}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12713,9 +12716,12 @@
       <c r="C33" s="9" t="s">
         <v>143</v>
       </c>
+      <c r="D33" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H33" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -12843,7 +12849,7 @@
       <c r="C41" s="40"/>
       <c r="D41" s="22">
         <f>COUNTA(D5:D40)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E41" s="22">
         <f t="shared" ref="E41:G41" si="1">COUNTA(E5:E40)</f>
@@ -12859,7 +12865,7 @@
       </c>
       <c r="H41" s="23">
         <f>COUNTIF(H5:H40,"X")</f>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -12893,11 +12899,11 @@
       </c>
       <c r="D46" s="10">
         <f>D45-D47</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E46" s="12">
         <f>D46/D45</f>
-        <v>0.44444444444444442</v>
+        <v>0.47222222222222221</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -12906,11 +12912,11 @@
       </c>
       <c r="D47" s="10">
         <f>H41</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E47" s="12">
         <f>D47/D45</f>
-        <v>0.55555555555555558</v>
+        <v>0.52777777777777779</v>
       </c>
     </row>
   </sheetData>
@@ -12931,8 +12937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F67FE634-56F6-4127-84CF-6C812025014A}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13645,8 +13651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581CE2C6-5A3B-4910-989B-A6ED716B8D89}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13792,9 +13798,12 @@
       <c r="C9" s="9" t="s">
         <v>189</v>
       </c>
+      <c r="D9" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -14306,7 +14315,7 @@
       <c r="C39" s="40"/>
       <c r="D39" s="22">
         <f>COUNTA(D5:D38)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E39" s="22">
         <f t="shared" ref="E39:G39" si="1">COUNTA(E5:E38)</f>
@@ -14322,7 +14331,7 @@
       </c>
       <c r="H39" s="23">
         <f>COUNTIF($H$5:$H$38,"X")</f>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -14356,11 +14365,11 @@
       </c>
       <c r="D44" s="10">
         <f>D43-D45</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E44" s="12">
         <f>D44/D43</f>
-        <v>0.76470588235294112</v>
+        <v>0.79411764705882348</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -14369,11 +14378,11 @@
       </c>
       <c r="D45" s="10">
         <f>H39</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E45" s="12">
         <f>D45/D43</f>
-        <v>0.23529411764705882</v>
+        <v>0.20588235294117646</v>
       </c>
     </row>
   </sheetData>
@@ -14394,7 +14403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75EE12D0-9DBC-4060-A74D-7E7E6A600169}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -15896,7 +15905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E26084B0-3C12-462B-B273-6776CCBE4AD2}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Version de listado de medios de comunicacion
nueva versión del archivo
</commit_message>
<xml_diff>
--- a/2020/listados/Listado de medios de comunicacion con estudiantes.xlsx
+++ b/2020/listados/Listado de medios de comunicacion con estudiantes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\GitHub\liceopatria.github.io\2020\listados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC2511A-C279-4A36-8CAB-D99016C44AE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BD29F5-495F-4F6F-883C-793DDEC1C5F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="1185" windowWidth="14400" windowHeight="10755" tabRatio="710" firstSheet="2" activeTab="11" xr2:uid="{50E3D567-1B3A-45B1-BFAB-81E44AF5B42C}"/>
+    <workbookView xWindow="3345" yWindow="2865" windowWidth="14400" windowHeight="10755" tabRatio="710" firstSheet="2" activeTab="11" xr2:uid="{50E3D567-1B3A-45B1-BFAB-81E44AF5B42C}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="15" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="518">
   <si>
     <t>Codigo</t>
   </si>
@@ -2823,7 +2823,7 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>27</c:v>
@@ -2844,7 +2844,7 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>32</c:v>
@@ -3015,7 +3015,7 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>7</c:v>
@@ -3036,7 +3036,7 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2</c:v>
@@ -3490,7 +3490,7 @@
                   <c:v>0.47222222222222221</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.48484848484848486</c:v>
+                  <c:v>0.51515151515151514</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.79411764705882348</c:v>
@@ -3511,7 +3511,7 @@
                   <c:v>0.59375</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.45454545454545453</c:v>
+                  <c:v>0.48484848484848486</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.94117647058823528</c:v>
@@ -3679,7 +3679,7 @@
                   <c:v>0.52777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.51515151515151514</c:v>
+                  <c:v>0.48484848484848486</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.20588235294117646</c:v>
@@ -3700,7 +3700,7 @@
                   <c:v>0.40625</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.54545454545454541</c:v>
+                  <c:v>0.51515151515151514</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>5.8823529411764705E-2</c:v>
@@ -5547,7 +5547,7 @@
       </c>
       <c r="E5" s="10">
         <f>'08-3'!D44</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F5" s="10">
         <f>'08-4'!D44</f>
@@ -5575,7 +5575,7 @@
       </c>
       <c r="L5" s="10">
         <f>'10-3'!D43</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M5" s="10">
         <f>'11-1'!D44</f>
@@ -5591,7 +5591,7 @@
       </c>
       <c r="P5" s="33">
         <f t="shared" ref="P5:P8" si="0">AVERAGE(B5:O5)</f>
-        <v>24.714285714285715</v>
+        <v>24.857142857142858</v>
       </c>
       <c r="Q5" s="33">
         <f t="shared" ref="Q5:Q8" si="1">MAX(B5:O5)</f>
@@ -5599,7 +5599,7 @@
       </c>
       <c r="R5" s="33">
         <f t="shared" ref="R5:R8" si="2">MIN(B5:O5)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
@@ -5620,7 +5620,7 @@
       </c>
       <c r="E6" s="10">
         <f>'08-3'!D45</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="10">
         <f>'08-4'!D45</f>
@@ -5648,7 +5648,7 @@
       </c>
       <c r="L6" s="10">
         <f>'10-3'!D44</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M6" s="10">
         <f>'11-1'!D45</f>
@@ -5664,7 +5664,7 @@
       </c>
       <c r="P6" s="33">
         <f t="shared" si="0"/>
-        <v>9.3571428571428577</v>
+        <v>9.2142857142857135</v>
       </c>
       <c r="Q6" s="33">
         <f t="shared" si="1"/>
@@ -5693,7 +5693,7 @@
       </c>
       <c r="E7" s="32">
         <f t="shared" si="3"/>
-        <v>0.48484848484848486</v>
+        <v>0.51515151515151514</v>
       </c>
       <c r="F7" s="32">
         <f t="shared" si="3"/>
@@ -5721,7 +5721,7 @@
       </c>
       <c r="L7" s="32">
         <f t="shared" si="3"/>
-        <v>0.45454545454545453</v>
+        <v>0.48484848484848486</v>
       </c>
       <c r="M7" s="32">
         <f t="shared" si="3"/>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="P7" s="34">
         <f t="shared" si="0"/>
-        <v>0.72880512053306157</v>
+        <v>0.73313412486206608</v>
       </c>
       <c r="Q7" s="34">
         <f t="shared" si="1"/>
@@ -5745,7 +5745,7 @@
       </c>
       <c r="R7" s="34">
         <f t="shared" si="2"/>
-        <v>0.45454545454545453</v>
+        <v>0.47222222222222221</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
@@ -5766,7 +5766,7 @@
       </c>
       <c r="E8" s="36">
         <f t="shared" si="4"/>
-        <v>0.51515151515151514</v>
+        <v>0.48484848484848486</v>
       </c>
       <c r="F8" s="36">
         <f t="shared" si="4"/>
@@ -5794,7 +5794,7 @@
       </c>
       <c r="L8" s="36">
         <f t="shared" si="4"/>
-        <v>0.54545454545454541</v>
+        <v>0.51515151515151514</v>
       </c>
       <c r="M8" s="36">
         <f t="shared" si="4"/>
@@ -5810,11 +5810,11 @@
       </c>
       <c r="P8" s="37">
         <f t="shared" si="0"/>
-        <v>0.27119487946693827</v>
+        <v>0.26686587513793392</v>
       </c>
       <c r="Q8" s="37">
         <f t="shared" si="1"/>
-        <v>0.54545454545454541</v>
+        <v>0.52777777777777779</v>
       </c>
       <c r="R8" s="37">
         <f t="shared" si="2"/>
@@ -7623,8 +7623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E6AB2A-DF13-43E5-8B37-FC6F541704E3}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7881,9 +7881,12 @@
       <c r="C16" s="9" t="s">
         <v>398</v>
       </c>
+      <c r="D16" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -8236,7 +8239,7 @@
       <c r="C38" s="40"/>
       <c r="D38" s="22">
         <f>COUNTA(D5:D37)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E38" s="22">
         <f t="shared" ref="E38:G38" si="1">COUNTA(E5:E37)</f>
@@ -8252,7 +8255,7 @@
       </c>
       <c r="H38" s="23">
         <f>COUNTIF(H5:H37,"X")</f>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -8286,11 +8289,11 @@
       </c>
       <c r="D43" s="10">
         <f>D42-D44</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E43" s="12">
         <f>D43/D42</f>
-        <v>0.45454545454545453</v>
+        <v>0.48484848484848486</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -8299,11 +8302,11 @@
       </c>
       <c r="D44" s="10">
         <f>H38</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E44" s="12">
         <f>D44/D42</f>
-        <v>0.54545454545454541</v>
+        <v>0.51515151515151514</v>
       </c>
     </row>
   </sheetData>
@@ -12950,7 +12953,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13326,9 +13329,12 @@
       <c r="C23" s="9" t="s">
         <v>169</v>
       </c>
+      <c r="D23" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H23" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -13564,7 +13570,7 @@
       <c r="C38" s="40"/>
       <c r="D38" s="22">
         <f>COUNTA(D5:D37)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E38" s="22">
         <f t="shared" ref="E38:G38" si="1">COUNTA(E5:E37)</f>
@@ -13580,7 +13586,7 @@
       </c>
       <c r="H38" s="23">
         <f>COUNTIF(H5:H37,"X")</f>
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -13625,11 +13631,11 @@
       </c>
       <c r="D44" s="10">
         <f>D43-D45</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E44" s="12">
         <f>D44/D43</f>
-        <v>0.48484848484848486</v>
+        <v>0.51515151515151514</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -13638,11 +13644,11 @@
       </c>
       <c r="D45" s="10">
         <f>H38</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E45" s="12">
         <f>D45/D43</f>
-        <v>0.51515151515151514</v>
+        <v>0.48484848484848486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Subida de versión de los archivos
</commit_message>
<xml_diff>
--- a/2020/listados/Listado de medios de comunicacion con estudiantes.xlsx
+++ b/2020/listados/Listado de medios de comunicacion con estudiantes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\GitHub\liceopatria.github.io\2020\listados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BD29F5-495F-4F6F-883C-793DDEC1C5F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683AD57B-BD14-4F61-94D5-22C963DC8E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3345" yWindow="2865" windowWidth="14400" windowHeight="10755" tabRatio="710" firstSheet="2" activeTab="11" xr2:uid="{50E3D567-1B3A-45B1-BFAB-81E44AF5B42C}"/>
+    <workbookView xWindow="3345" yWindow="2865" windowWidth="14400" windowHeight="10755" tabRatio="710" activeTab="1" xr2:uid="{50E3D567-1B3A-45B1-BFAB-81E44AF5B42C}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="15" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="518">
   <si>
     <t>Codigo</t>
   </si>
@@ -2814,7 +2814,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>30</c:v>
@@ -2829,7 +2829,7 @@
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>27</c:v>
@@ -3006,7 +3006,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -3021,7 +3021,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7</c:v>
@@ -3481,7 +3481,7 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.52500000000000002</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.88235294117647056</c:v>
@@ -3496,7 +3496,7 @@
                   <c:v>0.79411764705882348</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.79411764705882348</c:v>
+                  <c:v>0.82352941176470584</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.79411764705882348</c:v>
@@ -3670,7 +3670,7 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.47499999999999998</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.11764705882352941</c:v>
@@ -3685,7 +3685,7 @@
                   <c:v>0.20588235294117646</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.20588235294117646</c:v>
+                  <c:v>0.17647058823529413</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.20588235294117646</c:v>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="B5" s="10">
         <f>'06-1'!D50</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="10">
         <f>'08-1'!D44</f>
@@ -5555,7 +5555,7 @@
       </c>
       <c r="G5" s="10">
         <f>'09-1'!D44</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H5" s="10">
         <f>'09-2'!D44</f>
@@ -5591,7 +5591,7 @@
       </c>
       <c r="P5" s="33">
         <f t="shared" ref="P5:P8" si="0">AVERAGE(B5:O5)</f>
-        <v>24.857142857142858</v>
+        <v>25</v>
       </c>
       <c r="Q5" s="33">
         <f t="shared" ref="Q5:Q8" si="1">MAX(B5:O5)</f>
@@ -5608,7 +5608,7 @@
       </c>
       <c r="B6" s="10">
         <f>'06-1'!D51</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="10">
         <f>'08-1'!D45</f>
@@ -5628,7 +5628,7 @@
       </c>
       <c r="G6" s="10">
         <f>'09-1'!D45</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H6" s="10">
         <f>'09-2'!D45</f>
@@ -5664,7 +5664,7 @@
       </c>
       <c r="P6" s="33">
         <f t="shared" si="0"/>
-        <v>9.2142857142857135</v>
+        <v>9.0714285714285712</v>
       </c>
       <c r="Q6" s="33">
         <f t="shared" si="1"/>
@@ -5681,7 +5681,7 @@
       </c>
       <c r="B7" s="32">
         <f>B5/B4</f>
-        <v>0.52500000000000002</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C7" s="32">
         <f t="shared" ref="C7:O7" si="3">C5/C4</f>
@@ -5701,7 +5701,7 @@
       </c>
       <c r="G7" s="32">
         <f t="shared" si="3"/>
-        <v>0.79411764705882348</v>
+        <v>0.82352941176470584</v>
       </c>
       <c r="H7" s="32">
         <f t="shared" si="3"/>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="P7" s="34">
         <f t="shared" si="0"/>
-        <v>0.73313412486206608</v>
+        <v>0.7370206794839147</v>
       </c>
       <c r="Q7" s="34">
         <f t="shared" si="1"/>
@@ -5754,7 +5754,7 @@
       </c>
       <c r="B8" s="36">
         <f>B6/B4</f>
-        <v>0.47499999999999998</v>
+        <v>0.45</v>
       </c>
       <c r="C8" s="36">
         <f t="shared" ref="C8:O8" si="4">C6/C4</f>
@@ -5774,7 +5774,7 @@
       </c>
       <c r="G8" s="36">
         <f t="shared" si="4"/>
-        <v>0.20588235294117646</v>
+        <v>0.17647058823529413</v>
       </c>
       <c r="H8" s="36">
         <f t="shared" si="4"/>
@@ -5810,7 +5810,7 @@
       </c>
       <c r="P8" s="37">
         <f t="shared" si="0"/>
-        <v>0.26686587513793392</v>
+        <v>0.26297932051608519</v>
       </c>
       <c r="Q8" s="37">
         <f t="shared" si="1"/>
@@ -6167,7 +6167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE5E425-7606-4CA0-91F7-19ECFA2BFA71}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -7623,8 +7623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E6AB2A-DF13-43E5-8B37-FC6F541704E3}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8327,7 +8327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FF5F04-C5ED-4EA2-B9A1-243676970C03}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -9094,7 +9094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A71EA1-F646-4F3E-830E-E1FBC54465F3}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -9844,7 +9844,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10600,8 +10600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10776,9 +10776,12 @@
       <c r="C11" s="9" t="s">
         <v>9</v>
       </c>
+      <c r="D11" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -11335,7 +11338,7 @@
       <c r="C45" s="40"/>
       <c r="D45" s="22">
         <f>COUNTA(D5:D44)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E45" s="22">
         <f t="shared" ref="E45:G45" si="1">COUNTA(E5:E44)</f>
@@ -11351,7 +11354,7 @@
       </c>
       <c r="H45" s="23">
         <f>COUNTIF(H5:H44,"X")</f>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -11389,11 +11392,11 @@
       </c>
       <c r="D50" s="10">
         <f>D49-D51</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E50" s="12">
         <f>D50/$D$49</f>
-        <v>0.52500000000000002</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="51" spans="3:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -11402,11 +11405,11 @@
       </c>
       <c r="D51" s="10">
         <f>H45</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E51" s="12">
         <f>D51/$D$49</f>
-        <v>0.47499999999999998</v>
+        <v>0.45</v>
       </c>
     </row>
   </sheetData>
@@ -12953,7 +12956,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14422,7 +14425,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14966,9 +14969,12 @@
       <c r="C32" s="9" t="s">
         <v>246</v>
       </c>
+      <c r="D32" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -15084,7 +15090,7 @@
       <c r="C39" s="40"/>
       <c r="D39" s="22">
         <f>COUNTA(D5:D38)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E39" s="22">
         <f t="shared" ref="E39:G39" si="1">COUNTA(E5:E38)</f>
@@ -15100,7 +15106,7 @@
       </c>
       <c r="H39" s="23">
         <f>COUNTIF($H$5:$H$38,"X")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -15134,11 +15140,11 @@
       </c>
       <c r="D44" s="10">
         <f>D43-D45</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E44" s="12">
         <f>D44/D43</f>
-        <v>0.79411764705882348</v>
+        <v>0.82352941176470584</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -15147,11 +15153,11 @@
       </c>
       <c r="D45" s="10">
         <f>H39</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E45" s="12">
         <f>D45/D43</f>
-        <v>0.20588235294117646</v>
+        <v>0.17647058823529413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Versión de los archivos 20200506
</commit_message>
<xml_diff>
--- a/2020/listados/Listado de medios de comunicacion con estudiantes.xlsx
+++ b/2020/listados/Listado de medios de comunicacion con estudiantes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\GitHub\liceopatria.github.io\2020\listados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683AD57B-BD14-4F61-94D5-22C963DC8E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9BB3B2-EB12-46B6-A0EA-D98A6255B7EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3345" yWindow="2865" windowWidth="14400" windowHeight="10755" tabRatio="710" activeTab="1" xr2:uid="{50E3D567-1B3A-45B1-BFAB-81E44AF5B42C}"/>
+    <workbookView xWindow="3345" yWindow="2865" windowWidth="14400" windowHeight="10755" tabRatio="710" firstSheet="5" activeTab="12" xr2:uid="{50E3D567-1B3A-45B1-BFAB-81E44AF5B42C}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="15" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="518">
   <si>
     <t>Codigo</t>
   </si>
@@ -2814,7 +2814,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>30</c:v>
@@ -2823,7 +2823,7 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>27</c:v>
@@ -3006,7 +3006,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -3015,7 +3015,7 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>7</c:v>
@@ -3481,7 +3481,7 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.57499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.88235294117647056</c:v>
@@ -3490,7 +3490,7 @@
                   <c:v>0.47222222222222221</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.51515151515151514</c:v>
+                  <c:v>0.54545454545454541</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.79411764705882348</c:v>
@@ -3670,7 +3670,7 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.45</c:v>
+                  <c:v>0.42499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.11764705882352941</c:v>
@@ -3679,7 +3679,7 @@
                   <c:v>0.52777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.48484848484848486</c:v>
+                  <c:v>0.45454545454545453</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.20588235294117646</c:v>
@@ -5535,7 +5535,7 @@
       </c>
       <c r="B5" s="10">
         <f>'06-1'!D50</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="10">
         <f>'08-1'!D44</f>
@@ -5547,7 +5547,7 @@
       </c>
       <c r="E5" s="10">
         <f>'08-3'!D44</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5" s="10">
         <f>'08-4'!D44</f>
@@ -5591,7 +5591,7 @@
       </c>
       <c r="P5" s="33">
         <f t="shared" ref="P5:P8" si="0">AVERAGE(B5:O5)</f>
-        <v>25</v>
+        <v>25.142857142857142</v>
       </c>
       <c r="Q5" s="33">
         <f t="shared" ref="Q5:Q8" si="1">MAX(B5:O5)</f>
@@ -5608,7 +5608,7 @@
       </c>
       <c r="B6" s="10">
         <f>'06-1'!D51</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="10">
         <f>'08-1'!D45</f>
@@ -5620,7 +5620,7 @@
       </c>
       <c r="E6" s="10">
         <f>'08-3'!D45</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="10">
         <f>'08-4'!D45</f>
@@ -5664,7 +5664,7 @@
       </c>
       <c r="P6" s="33">
         <f t="shared" si="0"/>
-        <v>9.0714285714285712</v>
+        <v>8.9285714285714288</v>
       </c>
       <c r="Q6" s="33">
         <f t="shared" si="1"/>
@@ -5681,7 +5681,7 @@
       </c>
       <c r="B7" s="32">
         <f>B5/B4</f>
-        <v>0.55000000000000004</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="C7" s="32">
         <f t="shared" ref="C7:O7" si="3">C5/C4</f>
@@ -5693,7 +5693,7 @@
       </c>
       <c r="E7" s="32">
         <f t="shared" si="3"/>
-        <v>0.51515151515151514</v>
+        <v>0.54545454545454541</v>
       </c>
       <c r="F7" s="32">
         <f t="shared" si="3"/>
@@ -5737,7 +5737,7 @@
       </c>
       <c r="P7" s="34">
         <f t="shared" si="0"/>
-        <v>0.7370206794839147</v>
+        <v>0.74097089593413124</v>
       </c>
       <c r="Q7" s="34">
         <f t="shared" si="1"/>
@@ -5754,7 +5754,7 @@
       </c>
       <c r="B8" s="36">
         <f>B6/B4</f>
-        <v>0.45</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="C8" s="36">
         <f t="shared" ref="C8:O8" si="4">C6/C4</f>
@@ -5766,7 +5766,7 @@
       </c>
       <c r="E8" s="36">
         <f t="shared" si="4"/>
-        <v>0.48484848484848486</v>
+        <v>0.45454545454545453</v>
       </c>
       <c r="F8" s="36">
         <f t="shared" si="4"/>
@@ -5810,7 +5810,7 @@
       </c>
       <c r="P8" s="37">
         <f t="shared" si="0"/>
-        <v>0.26297932051608519</v>
+        <v>0.25902910406586871</v>
       </c>
       <c r="Q8" s="37">
         <f t="shared" si="1"/>
@@ -8327,8 +8327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FF5F04-C5ED-4EA2-B9A1-243676970C03}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10600,8 +10600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11310,9 +11310,12 @@
       <c r="C43" s="9" t="s">
         <v>41</v>
       </c>
+      <c r="D43" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H43" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -11338,7 +11341,7 @@
       <c r="C45" s="40"/>
       <c r="D45" s="22">
         <f>COUNTA(D5:D44)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E45" s="22">
         <f t="shared" ref="E45:G45" si="1">COUNTA(E5:E44)</f>
@@ -11354,7 +11357,7 @@
       </c>
       <c r="H45" s="23">
         <f>COUNTIF(H5:H44,"X")</f>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -11392,11 +11395,11 @@
       </c>
       <c r="D50" s="10">
         <f>D49-D51</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E50" s="12">
         <f>D50/$D$49</f>
-        <v>0.55000000000000004</v>
+        <v>0.57499999999999996</v>
       </c>
     </row>
     <row r="51" spans="3:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -11405,11 +11408,11 @@
       </c>
       <c r="D51" s="10">
         <f>H45</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E51" s="12">
         <f>D51/$D$49</f>
-        <v>0.45</v>
+        <v>0.42499999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -12955,8 +12958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F67FE634-56F6-4127-84CF-6C812025014A}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13029,9 +13032,12 @@
       <c r="C5" s="9" t="s">
         <v>151</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H5" s="4" t="str">
         <f>IF(COUNTA(D5:G5)=0,"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -13573,7 +13579,7 @@
       <c r="C38" s="40"/>
       <c r="D38" s="22">
         <f>COUNTA(D5:D37)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E38" s="22">
         <f t="shared" ref="E38:G38" si="1">COUNTA(E5:E37)</f>
@@ -13589,7 +13595,7 @@
       </c>
       <c r="H38" s="23">
         <f>COUNTIF(H5:H37,"X")</f>
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -13634,11 +13640,11 @@
       </c>
       <c r="D44" s="10">
         <f>D43-D45</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E44" s="12">
         <f>D44/D43</f>
-        <v>0.51515151515151514</v>
+        <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -13647,11 +13653,11 @@
       </c>
       <c r="D45" s="10">
         <f>H38</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E45" s="12">
         <f>D45/D43</f>
-        <v>0.48484848484848486</v>
+        <v>0.45454545454545453</v>
       </c>
     </row>
   </sheetData>

</xml_diff>